<commit_message>
FInished PE analysis, added protein analysis markdown, added bootstrapping markdown
Started working on protein, finished graph products for PE.
</commit_message>
<xml_diff>
--- a/PE/Input PE/pe3_weights_id.xlsx
+++ b/PE/Input PE/pe3_weights_id.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\ACES\Dissy\analysis\PE\Input PE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trevo\OneDrive\Documents\GitHub\TEdissy_analysis\PE\Input PE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614D2255-6DCF-4CF4-93AE-493BFC419AF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C195286D-82BA-477E-9514-6406EB6610E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{3EEF7A1E-F4AB-451B-9449-A4DC2C438512}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9600" windowHeight="10200" xr2:uid="{3EEF7A1E-F4AB-451B-9449-A4DC2C438512}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="106">
   <si>
     <t>Lab_40</t>
   </si>
@@ -290,42 +290,6 @@
     <t>D05</t>
   </si>
   <si>
-    <t>juice ilo</t>
-  </si>
-  <si>
-    <t>D06</t>
-  </si>
-  <si>
-    <t>D07</t>
-  </si>
-  <si>
-    <t>D08</t>
-  </si>
-  <si>
-    <t>juice fresh  R2</t>
-  </si>
-  <si>
-    <t>A13</t>
-  </si>
-  <si>
-    <t>D09</t>
-  </si>
-  <si>
-    <t>juice fresh R2</t>
-  </si>
-  <si>
-    <t>A14</t>
-  </si>
-  <si>
-    <t>D10</t>
-  </si>
-  <si>
-    <t>A15</t>
-  </si>
-  <si>
-    <t>D11</t>
-  </si>
-  <si>
     <t>A16</t>
   </si>
   <si>
@@ -335,6 +299,48 @@
     <t>E01</t>
   </si>
   <si>
+    <t>Blank_04</t>
+  </si>
+  <si>
+    <t>H09</t>
+  </si>
+  <si>
+    <t>Blank_05</t>
+  </si>
+  <si>
+    <t>Blank_06</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>sample weight</t>
+  </si>
+  <si>
+    <t>Tray well</t>
+  </si>
+  <si>
+    <t>plate well</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>Lab_71</t>
+  </si>
+  <si>
+    <t>Lab_72</t>
+  </si>
+  <si>
+    <t>Lab_73</t>
+  </si>
+  <si>
+    <t>Lab_74</t>
+  </si>
+  <si>
+    <t>Lab_75</t>
+  </si>
+  <si>
     <t>E02</t>
   </si>
   <si>
@@ -347,211 +353,7 @@
     <t>E05</t>
   </si>
   <si>
-    <t>Ilo oven dry R01</t>
-  </si>
-  <si>
-    <t>E6</t>
-  </si>
-  <si>
-    <t>E09</t>
-  </si>
-  <si>
-    <t>E7</t>
-  </si>
-  <si>
-    <t>E10</t>
-  </si>
-  <si>
-    <t>E8</t>
-  </si>
-  <si>
-    <t>E11</t>
-  </si>
-  <si>
-    <t>Lima R01 oven dry</t>
-  </si>
-  <si>
-    <t>E15</t>
-  </si>
-  <si>
-    <t>F06</t>
-  </si>
-  <si>
-    <t>E16</t>
-  </si>
-  <si>
-    <t>F07</t>
-  </si>
-  <si>
-    <t>F01</t>
-  </si>
-  <si>
-    <t>F08</t>
-  </si>
-  <si>
-    <t>Lima R02 oven dry</t>
-  </si>
-  <si>
-    <t>F09</t>
-  </si>
-  <si>
-    <t>F10</t>
-  </si>
-  <si>
-    <t>F11</t>
-  </si>
-  <si>
-    <t>Lima R03 oven dry</t>
-  </si>
-  <si>
-    <t>E12</t>
-  </si>
-  <si>
-    <t>F12</t>
-  </si>
-  <si>
-    <t>E13</t>
-  </si>
-  <si>
-    <t>G01</t>
-  </si>
-  <si>
-    <t>E14</t>
-  </si>
-  <si>
-    <t>G02</t>
-  </si>
-  <si>
-    <t>Ilo oven dry R02</t>
-  </si>
-  <si>
-    <t>F02</t>
-  </si>
-  <si>
-    <t>F03</t>
-  </si>
-  <si>
-    <t>F04</t>
-  </si>
-  <si>
-    <t>F05</t>
-  </si>
-  <si>
-    <t>Ilo freeze dry R01</t>
-  </si>
-  <si>
-    <t>G03</t>
-  </si>
-  <si>
-    <t>G04</t>
-  </si>
-  <si>
-    <t>G05</t>
-  </si>
-  <si>
-    <t>Ilo freeze dry R02</t>
-  </si>
-  <si>
-    <t>G06</t>
-  </si>
-  <si>
-    <t>G07</t>
-  </si>
-  <si>
-    <t>F13</t>
-  </si>
-  <si>
-    <t>G08</t>
-  </si>
-  <si>
-    <t>Ilo freeze dry R03</t>
-  </si>
-  <si>
-    <t>F14</t>
-  </si>
-  <si>
-    <t>G09</t>
-  </si>
-  <si>
-    <t>F15</t>
-  </si>
-  <si>
-    <t>F16</t>
-  </si>
-  <si>
-    <t>Lima R01 freeze dry</t>
-  </si>
-  <si>
-    <t>H01</t>
-  </si>
-  <si>
-    <t>H02</t>
-  </si>
-  <si>
-    <t>Lima R02 freeze dry</t>
-  </si>
-  <si>
-    <t>H03</t>
-  </si>
-  <si>
-    <t>H04</t>
-  </si>
-  <si>
-    <t>H05</t>
-  </si>
-  <si>
-    <t>Lima R03 freeze dry</t>
-  </si>
-  <si>
-    <t>H06</t>
-  </si>
-  <si>
-    <t>H07</t>
-  </si>
-  <si>
-    <t>H08</t>
-  </si>
-  <si>
-    <t>Blank_04</t>
-  </si>
-  <si>
-    <t>H09</t>
-  </si>
-  <si>
-    <t>Blank_05</t>
-  </si>
-  <si>
-    <t>Blank_06</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>sample weight</t>
-  </si>
-  <si>
-    <t>Tray well</t>
-  </si>
-  <si>
-    <t>plate well</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
     <t>Lab_70</t>
-  </si>
-  <si>
-    <t>Lab_71</t>
-  </si>
-  <si>
-    <t>Lab_72</t>
-  </si>
-  <si>
-    <t>Lab_73</t>
-  </si>
-  <si>
-    <t>Lab_74</t>
   </si>
 </sst>
 </file>
@@ -941,32 +743,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4CE8875-D7F5-41D2-9F74-F229126DDF3C}">
-  <dimension ref="A1:E93"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="27.1796875" customWidth="1"/>
     <col min="5" max="5" width="14.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>162</v>
+        <v>91</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>163</v>
+        <v>92</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>164</v>
+        <v>93</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>165</v>
+        <v>94</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>166</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -1513,12 +1316,12 @@
         <v>45792</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>167</v>
+        <v>105</v>
       </c>
       <c r="B34" s="1">
-        <v>199.7</v>
+        <v>16.974499999999999</v>
       </c>
       <c r="C34" t="s">
         <v>2</v>
@@ -1530,12 +1333,12 @@
         <v>45792</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>167</v>
+        <v>105</v>
       </c>
       <c r="B35">
-        <v>208.4</v>
+        <v>17.714000000000002</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
@@ -1547,12 +1350,12 @@
         <v>45792</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>167</v>
+        <v>105</v>
       </c>
       <c r="B36" s="1">
-        <v>15.895000000000001</v>
+        <v>15.895</v>
       </c>
       <c r="C36" t="s">
         <v>6</v>
@@ -1566,7 +1369,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>168</v>
+        <v>96</v>
       </c>
       <c r="B37" s="1">
         <v>16.32</v>
@@ -1583,7 +1386,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>168</v>
+        <v>96</v>
       </c>
       <c r="B38" s="1">
         <v>21.666500000000003</v>
@@ -1600,7 +1403,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>168</v>
+        <v>96</v>
       </c>
       <c r="B39" s="1">
         <v>20.536000000000001</v>
@@ -1617,7 +1420,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>169</v>
+        <v>97</v>
       </c>
       <c r="B40" s="1">
         <v>15.546500000000002</v>
@@ -1634,7 +1437,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>169</v>
+        <v>97</v>
       </c>
       <c r="B41" s="1">
         <v>18.955000000000002</v>
@@ -1651,7 +1454,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>169</v>
+        <v>97</v>
       </c>
       <c r="B42" s="1">
         <v>18.768000000000001</v>
@@ -1668,13 +1471,13 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
+        <v>98</v>
+      </c>
+      <c r="B43" s="1">
+        <v>18.028500000000001</v>
+      </c>
+      <c r="C43" t="s">
         <v>84</v>
-      </c>
-      <c r="B43" s="1">
-        <v>15.2745</v>
-      </c>
-      <c r="C43" t="s">
-        <v>23</v>
       </c>
       <c r="D43" t="s">
         <v>85</v>
@@ -1685,13 +1488,13 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="B44" s="1">
-        <v>21.080000000000002</v>
+        <v>14.637</v>
       </c>
       <c r="C44" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D44" t="s">
         <v>86</v>
@@ -1702,16 +1505,16 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="B45" s="1">
-        <v>19.1845</v>
+        <v>19.065500000000004</v>
       </c>
       <c r="C45" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D45" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="E45" s="2">
         <v>45792</v>
@@ -1719,16 +1522,16 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="B46" s="1">
-        <v>19.057000000000002</v>
+        <v>20.000500000000002</v>
       </c>
       <c r="C46" t="s">
-        <v>89</v>
+        <v>34</v>
       </c>
       <c r="D46" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="E46" s="2">
         <v>45792</v>
@@ -1736,16 +1539,16 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="B47" s="1">
-        <v>14.076000000000001</v>
+        <v>16.234999999999999</v>
       </c>
       <c r="C47" t="s">
-        <v>92</v>
+        <v>37</v>
       </c>
       <c r="D47" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="E47" s="2">
         <v>45792</v>
@@ -1753,16 +1556,16 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="B48" s="1">
-        <v>13.770000000000001</v>
+        <v>15.529500000000001</v>
       </c>
       <c r="C48" t="s">
-        <v>94</v>
+        <v>39</v>
       </c>
       <c r="D48" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="E48" s="2">
         <v>45792</v>
@@ -1770,16 +1573,13 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>170</v>
-      </c>
-      <c r="B49" s="1">
-        <v>18.028500000000001</v>
+        <v>87</v>
       </c>
       <c r="C49" t="s">
-        <v>96</v>
+        <v>22</v>
       </c>
       <c r="D49" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="E49" s="2">
         <v>45792</v>
@@ -1787,16 +1587,13 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>170</v>
-      </c>
-      <c r="B50" s="1">
-        <v>14.637</v>
+        <v>89</v>
       </c>
       <c r="C50" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D50" t="s">
-        <v>98</v>
+        <v>59</v>
       </c>
       <c r="E50" s="2">
         <v>45792</v>
@@ -1804,723 +1601,15 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>170</v>
-      </c>
-      <c r="B51" s="1">
-        <v>19.065500000000004</v>
+        <v>90</v>
       </c>
       <c r="C51" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D51" t="s">
-        <v>99</v>
+        <v>61</v>
       </c>
       <c r="E51" s="2">
-        <v>45792</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
-        <v>171</v>
-      </c>
-      <c r="B52" s="1">
-        <v>20.000500000000002</v>
-      </c>
-      <c r="C52" t="s">
-        <v>34</v>
-      </c>
-      <c r="D52" t="s">
-        <v>100</v>
-      </c>
-      <c r="E52" s="2">
-        <v>45792</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
-        <v>171</v>
-      </c>
-      <c r="B53" s="1">
-        <v>16.234999999999999</v>
-      </c>
-      <c r="C53" t="s">
-        <v>37</v>
-      </c>
-      <c r="D53" t="s">
-        <v>101</v>
-      </c>
-      <c r="E53" s="2">
-        <v>45792</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
-        <v>171</v>
-      </c>
-      <c r="B54" s="1">
-        <v>15.529500000000001</v>
-      </c>
-      <c r="C54" t="s">
-        <v>39</v>
-      </c>
-      <c r="D54" t="s">
-        <v>102</v>
-      </c>
-      <c r="E54" s="2">
-        <v>45792</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
-        <v>103</v>
-      </c>
-      <c r="B55">
-        <v>24.9</v>
-      </c>
-      <c r="C55" t="s">
-        <v>104</v>
-      </c>
-      <c r="D55" t="s">
-        <v>105</v>
-      </c>
-      <c r="E55" s="2">
-        <v>45792</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
-        <v>103</v>
-      </c>
-      <c r="B56">
-        <v>26.6</v>
-      </c>
-      <c r="C56" t="s">
-        <v>106</v>
-      </c>
-      <c r="D56" t="s">
-        <v>107</v>
-      </c>
-      <c r="E56" s="2">
-        <v>45792</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
-        <v>103</v>
-      </c>
-      <c r="B57">
-        <v>25.1</v>
-      </c>
-      <c r="C57" t="s">
-        <v>108</v>
-      </c>
-      <c r="D57" t="s">
-        <v>109</v>
-      </c>
-      <c r="E57" s="2">
-        <v>45792</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
-        <v>110</v>
-      </c>
-      <c r="B58" s="1">
-        <v>27.9</v>
-      </c>
-      <c r="C58" t="s">
-        <v>111</v>
-      </c>
-      <c r="D58" t="s">
-        <v>112</v>
-      </c>
-      <c r="E58" s="2">
-        <v>45792</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
-        <v>110</v>
-      </c>
-      <c r="B59">
-        <v>23.5</v>
-      </c>
-      <c r="C59" t="s">
-        <v>113</v>
-      </c>
-      <c r="D59" t="s">
-        <v>114</v>
-      </c>
-      <c r="E59" s="2">
-        <v>45792</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
-        <v>110</v>
-      </c>
-      <c r="B60">
-        <v>24.1</v>
-      </c>
-      <c r="C60" t="s">
-        <v>115</v>
-      </c>
-      <c r="D60" t="s">
-        <v>116</v>
-      </c>
-      <c r="E60" s="2">
-        <v>45792</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
-        <v>117</v>
-      </c>
-      <c r="B61" s="1">
-        <v>26.7</v>
-      </c>
-      <c r="C61" t="s">
-        <v>105</v>
-      </c>
-      <c r="D61" t="s">
-        <v>118</v>
-      </c>
-      <c r="E61" s="2">
-        <v>45792</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
-        <v>117</v>
-      </c>
-      <c r="B62" s="1">
-        <v>22.1</v>
-      </c>
-      <c r="C62" t="s">
-        <v>107</v>
-      </c>
-      <c r="D62" t="s">
-        <v>119</v>
-      </c>
-      <c r="E62" s="2">
-        <v>45792</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A63" t="s">
-        <v>117</v>
-      </c>
-      <c r="B63" s="1">
-        <v>24.1</v>
-      </c>
-      <c r="C63" t="s">
-        <v>109</v>
-      </c>
-      <c r="D63" t="s">
-        <v>120</v>
-      </c>
-      <c r="E63" s="2">
-        <v>45792</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A64" t="s">
-        <v>121</v>
-      </c>
-      <c r="B64" s="1">
-        <v>25.6</v>
-      </c>
-      <c r="C64" t="s">
-        <v>122</v>
-      </c>
-      <c r="D64" t="s">
-        <v>123</v>
-      </c>
-      <c r="E64" s="2">
-        <v>45792</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A65" t="s">
-        <v>121</v>
-      </c>
-      <c r="B65" s="1">
-        <v>26.5</v>
-      </c>
-      <c r="C65" t="s">
-        <v>124</v>
-      </c>
-      <c r="D65" t="s">
-        <v>125</v>
-      </c>
-      <c r="E65" s="2">
-        <v>45792</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A66" t="s">
-        <v>121</v>
-      </c>
-      <c r="B66" s="1">
-        <v>23.2</v>
-      </c>
-      <c r="C66" t="s">
-        <v>126</v>
-      </c>
-      <c r="D66" t="s">
-        <v>127</v>
-      </c>
-      <c r="E66" s="2">
-        <v>45792</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A67" t="s">
-        <v>128</v>
-      </c>
-      <c r="B67" s="1">
-        <v>21.8</v>
-      </c>
-      <c r="C67" t="s">
-        <v>129</v>
-      </c>
-      <c r="D67" t="s">
-        <v>122</v>
-      </c>
-      <c r="E67" s="2">
-        <v>45792</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A68" t="s">
-        <v>128</v>
-      </c>
-      <c r="B68" s="1">
-        <v>27.4</v>
-      </c>
-      <c r="C68" t="s">
-        <v>130</v>
-      </c>
-      <c r="D68" t="s">
-        <v>115</v>
-      </c>
-      <c r="E68" s="2">
-        <v>45792</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A69" t="s">
-        <v>128</v>
-      </c>
-      <c r="B69" s="1">
-        <v>25.3</v>
-      </c>
-      <c r="C69" t="s">
-        <v>131</v>
-      </c>
-      <c r="D69" t="s">
-        <v>129</v>
-      </c>
-      <c r="E69" s="2">
-        <v>45792</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A70" t="s">
-        <v>128</v>
-      </c>
-      <c r="B70" s="1">
-        <v>23.2</v>
-      </c>
-      <c r="C70" t="s">
-        <v>132</v>
-      </c>
-      <c r="D70" t="s">
-        <v>130</v>
-      </c>
-      <c r="E70" s="2">
-        <v>45792</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A71" t="s">
-        <v>128</v>
-      </c>
-      <c r="B71" s="1">
-        <v>27.3</v>
-      </c>
-      <c r="C71" t="s">
-        <v>112</v>
-      </c>
-      <c r="D71" t="s">
-        <v>131</v>
-      </c>
-      <c r="E71" s="2">
-        <v>45792</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A72" t="s">
-        <v>128</v>
-      </c>
-      <c r="B72" s="1">
-        <v>23.8</v>
-      </c>
-      <c r="C72" t="s">
-        <v>114</v>
-      </c>
-      <c r="D72" t="s">
-        <v>132</v>
-      </c>
-      <c r="E72" s="2">
-        <v>45792</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A73" t="s">
-        <v>133</v>
-      </c>
-      <c r="B73" s="1">
-        <v>24.6</v>
-      </c>
-      <c r="C73" t="s">
-        <v>116</v>
-      </c>
-      <c r="D73" t="s">
-        <v>134</v>
-      </c>
-      <c r="E73" s="2">
-        <v>45792</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A74" t="s">
-        <v>133</v>
-      </c>
-      <c r="B74" s="1">
-        <v>22.6</v>
-      </c>
-      <c r="C74" t="s">
-        <v>118</v>
-      </c>
-      <c r="D74" t="s">
-        <v>135</v>
-      </c>
-      <c r="E74" s="2">
-        <v>45792</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A75" t="s">
-        <v>133</v>
-      </c>
-      <c r="B75" s="1">
-        <v>26</v>
-      </c>
-      <c r="C75" t="s">
-        <v>119</v>
-      </c>
-      <c r="D75" t="s">
-        <v>136</v>
-      </c>
-      <c r="E75" s="2">
-        <v>45792</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A76" t="s">
-        <v>137</v>
-      </c>
-      <c r="B76" s="1">
-        <v>23.3</v>
-      </c>
-      <c r="C76" t="s">
-        <v>120</v>
-      </c>
-      <c r="D76" t="s">
-        <v>138</v>
-      </c>
-      <c r="E76" s="2">
-        <v>45792</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A77" t="s">
-        <v>137</v>
-      </c>
-      <c r="B77" s="1">
-        <v>22</v>
-      </c>
-      <c r="C77" t="s">
-        <v>123</v>
-      </c>
-      <c r="D77" t="s">
-        <v>139</v>
-      </c>
-      <c r="E77" s="2">
-        <v>45792</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A78" t="s">
-        <v>137</v>
-      </c>
-      <c r="B78" s="1">
-        <v>25.7</v>
-      </c>
-      <c r="C78" t="s">
-        <v>140</v>
-      </c>
-      <c r="D78" t="s">
-        <v>141</v>
-      </c>
-      <c r="E78" s="2">
-        <v>45792</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A79" t="s">
-        <v>142</v>
-      </c>
-      <c r="B79" s="1">
-        <v>22.7</v>
-      </c>
-      <c r="C79" t="s">
-        <v>143</v>
-      </c>
-      <c r="D79" t="s">
-        <v>144</v>
-      </c>
-      <c r="E79" s="2">
-        <v>45792</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A80" t="s">
-        <v>142</v>
-      </c>
-      <c r="B80" s="1">
-        <v>25.3</v>
-      </c>
-      <c r="C80" t="s">
-        <v>145</v>
-      </c>
-      <c r="D80" t="s">
-        <v>22</v>
-      </c>
-      <c r="E80" s="2">
-        <v>45792</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A81" t="s">
-        <v>142</v>
-      </c>
-      <c r="B81" s="1">
-        <v>24.9</v>
-      </c>
-      <c r="C81" t="s">
-        <v>146</v>
-      </c>
-      <c r="D81" t="s">
-        <v>24</v>
-      </c>
-      <c r="E81" s="2">
-        <v>45792</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A82" t="s">
-        <v>147</v>
-      </c>
-      <c r="B82" s="1">
-        <v>27.6</v>
-      </c>
-      <c r="C82" t="s">
-        <v>125</v>
-      </c>
-      <c r="D82" t="s">
-        <v>26</v>
-      </c>
-      <c r="E82" s="2">
-        <v>45792</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A83" t="s">
-        <v>147</v>
-      </c>
-      <c r="B83" s="1">
-        <v>26.1</v>
-      </c>
-      <c r="C83" t="s">
-        <v>127</v>
-      </c>
-      <c r="D83" t="s">
-        <v>148</v>
-      </c>
-      <c r="E83" s="2">
-        <v>45792</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A84" t="s">
-        <v>147</v>
-      </c>
-      <c r="B84" s="1">
-        <v>25.6</v>
-      </c>
-      <c r="C84" t="s">
-        <v>134</v>
-      </c>
-      <c r="D84" t="s">
-        <v>149</v>
-      </c>
-      <c r="E84" s="2">
-        <v>45792</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A85" t="s">
-        <v>150</v>
-      </c>
-      <c r="B85" s="1">
-        <v>24.2</v>
-      </c>
-      <c r="C85" t="s">
-        <v>135</v>
-      </c>
-      <c r="D85" t="s">
-        <v>151</v>
-      </c>
-      <c r="E85" s="2">
-        <v>45792</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A86" t="s">
-        <v>150</v>
-      </c>
-      <c r="B86" s="1">
-        <v>22.6</v>
-      </c>
-      <c r="C86" t="s">
-        <v>136</v>
-      </c>
-      <c r="D86" t="s">
-        <v>152</v>
-      </c>
-      <c r="E86" s="2">
-        <v>45792</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A87" t="s">
-        <v>150</v>
-      </c>
-      <c r="B87" s="1">
-        <v>25.8</v>
-      </c>
-      <c r="C87" t="s">
-        <v>138</v>
-      </c>
-      <c r="D87" t="s">
-        <v>153</v>
-      </c>
-      <c r="E87" s="2">
-        <v>45792</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A88" t="s">
-        <v>154</v>
-      </c>
-      <c r="B88" s="1">
-        <v>25.7</v>
-      </c>
-      <c r="C88" t="s">
-        <v>139</v>
-      </c>
-      <c r="D88" t="s">
-        <v>155</v>
-      </c>
-      <c r="E88" s="2">
-        <v>45792</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A89" t="s">
-        <v>154</v>
-      </c>
-      <c r="B89" s="1">
-        <v>25.3</v>
-      </c>
-      <c r="C89" t="s">
-        <v>141</v>
-      </c>
-      <c r="D89" t="s">
-        <v>156</v>
-      </c>
-      <c r="E89" s="2">
-        <v>45792</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A90" t="s">
-        <v>154</v>
-      </c>
-      <c r="B90" s="1">
-        <v>23.5</v>
-      </c>
-      <c r="C90" t="s">
-        <v>144</v>
-      </c>
-      <c r="D90" t="s">
-        <v>157</v>
-      </c>
-      <c r="E90" s="2">
-        <v>45792</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A91" t="s">
-        <v>158</v>
-      </c>
-      <c r="C91" t="s">
-        <v>22</v>
-      </c>
-      <c r="D91" t="s">
-        <v>159</v>
-      </c>
-      <c r="E91" s="2">
-        <v>45792</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A92" t="s">
-        <v>160</v>
-      </c>
-      <c r="C92" t="s">
-        <v>24</v>
-      </c>
-      <c r="D92" t="s">
-        <v>59</v>
-      </c>
-      <c r="E92" s="2">
-        <v>45792</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A93" t="s">
-        <v>161</v>
-      </c>
-      <c r="C93" t="s">
-        <v>26</v>
-      </c>
-      <c r="D93" t="s">
-        <v>61</v>
-      </c>
-      <c r="E93" s="2">
         <v>45792</v>
       </c>
     </row>

</xml_diff>